<commit_message>
bug: data set seems strange
</commit_message>
<xml_diff>
--- a/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
+++ b/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephan\Desktop\repos\wt_modeling\Drafts\lmfit_biocatalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMalz\Desktop\Repos\wt_modeling\Drafts\lmfit_biocatalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8493BB65-EFA0-4C78-B3AD-2FB8A0B98283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F90B7D-8833-47D2-9337-5BAB23169528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
+    <workbookView xWindow="58815" yWindow="10155" windowWidth="15705" windowHeight="9720" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -472,18 +472,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B764C8B-F5EC-4044-AE1A-6A1FF61ED92C}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>8.736349453978158E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -552,7 +552,7 @@
         <v>2.937077483099324</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -575,7 +575,7 @@
         <v>3.6235049401976078</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -598,95 +598,72 @@
         <v>10.799791991679667</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="B6">
-        <v>11.326424870466321</v>
+        <v>4.9706390328151979</v>
       </c>
       <c r="C6" s="4">
-        <v>68.722272317403068</v>
+        <v>52.109708446047499</v>
       </c>
       <c r="D6">
-        <v>6.4940197607904322</v>
+        <v>9.0629225169006755</v>
       </c>
       <c r="E6">
-        <v>4.9533678756476691</v>
+        <v>3.4162348877374789</v>
       </c>
       <c r="F6" s="4">
-        <v>42.317102494739999</v>
+        <v>54.099489029155393</v>
       </c>
       <c r="G6">
-        <v>16.083203328133127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>32.079043161726467</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="B7">
-        <v>4.9706390328151979</v>
+        <v>7.3886010362694305</v>
       </c>
       <c r="C7" s="4">
-        <v>52.109708446047499</v>
+        <v>51.370303576795912</v>
       </c>
       <c r="D7">
-        <v>9.0629225169006755</v>
+        <v>12.328653146125845</v>
       </c>
       <c r="E7">
-        <v>3.4162348877374789</v>
+        <v>2.9671848013816917</v>
       </c>
       <c r="F7" s="4">
-        <v>54.099489029155393</v>
+        <v>36.492034866245866</v>
       </c>
       <c r="G7">
-        <v>32.079043161726467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>360</v>
-      </c>
-      <c r="B8">
-        <v>7.3886010362694305</v>
-      </c>
-      <c r="C8" s="4">
-        <v>51.370303576795912</v>
-      </c>
-      <c r="D8">
-        <v>12.328653146125845</v>
-      </c>
-      <c r="E8">
-        <v>2.9671848013816917</v>
-      </c>
-      <c r="F8" s="4">
-        <v>36.492034866245866</v>
-      </c>
-      <c r="G8">
         <v>24.205928237129484</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>1440</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B8" s="3">
         <v>3.6407599309153711</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C8" s="5">
         <v>47.955816050495947</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D8" s="6">
         <v>13.051482059282371</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E8" s="3">
         <v>1.585492227979274</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F8" s="5">
         <v>43.44123835287045</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G8" s="6">
         <v>32.786271450858031</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug: model doesn't fit
</commit_message>
<xml_diff>
--- a/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
+++ b/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMalz\Desktop\Repos\wt_modeling\Drafts\lmfit_biocatalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F90B7D-8833-47D2-9337-5BAB23169528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E6F62A-7FC8-455E-AE4F-DAFC47B5D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58815" yWindow="10155" windowWidth="15705" windowHeight="9720" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
+    <workbookView xWindow="58290" yWindow="11325" windowWidth="15705" windowHeight="9720" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -62,10 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,19 +111,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -146,18 +139,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -472,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B764C8B-F5EC-4044-AE1A-6A1FF61ED92C}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,22 +518,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>96.594127806563009</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="7">
+        <v>118.42487046632124</v>
+      </c>
+      <c r="C2" s="9">
         <v>0.14697926059513075</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>8.736349453978158E-2</v>
       </c>
       <c r="E2">
         <v>132.84628670120895</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>0.14697926059513075</v>
       </c>
       <c r="G2">
@@ -530,22 +541,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>15</v>
       </c>
-      <c r="B3">
-        <v>59.927461139896366</v>
-      </c>
-      <c r="C3" s="4">
-        <v>44.956116621581003</v>
-      </c>
-      <c r="D3">
-        <v>8.736349453978158E-2</v>
+      <c r="B3" s="7">
+        <v>34.936096718480137</v>
+      </c>
+      <c r="C3" s="9">
+        <v>21.932371505861141</v>
+      </c>
+      <c r="D3" s="7">
+        <v>16.15600624024961</v>
       </c>
       <c r="E3">
         <v>37.146804835924009</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>42.250976856026455</v>
       </c>
       <c r="G3">
@@ -553,22 +564,22 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>32.483592400690846</v>
-      </c>
-      <c r="C4" s="4">
-        <v>52.241959723474615</v>
-      </c>
-      <c r="D4">
-        <v>1.2522100884035361</v>
+      <c r="B4" s="7">
+        <v>12.690846286701209</v>
+      </c>
+      <c r="C4" s="9">
+        <v>19.684099789600243</v>
+      </c>
+      <c r="D4" s="7">
+        <v>41.751430057202278</v>
       </c>
       <c r="E4">
         <v>22.656303972366146</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>46.116321009918842</v>
       </c>
       <c r="G4">
@@ -576,22 +587,22 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>60</v>
       </c>
-      <c r="B5">
-        <v>14.21070811744387</v>
-      </c>
-      <c r="C5" s="4">
-        <v>50.035767959122332</v>
-      </c>
-      <c r="D5">
-        <v>2.7706708268330726</v>
+      <c r="B5" s="7">
+        <v>6.3350604490500855</v>
+      </c>
+      <c r="C5" s="9">
+        <v>11.424406372107002</v>
+      </c>
+      <c r="D5" s="7">
+        <v>54.491939677587091</v>
       </c>
       <c r="E5">
         <v>11.930915371329879</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>44.421100090171329</v>
       </c>
       <c r="G5">
@@ -599,22 +610,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>260</v>
-      </c>
-      <c r="B6">
-        <v>4.9706390328151979</v>
-      </c>
-      <c r="C6" s="4">
-        <v>52.109708446047499</v>
-      </c>
-      <c r="D6">
-        <v>9.0629225169006755</v>
+      <c r="A6" s="5">
+        <v>120</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4.7288428324697742</v>
+      </c>
+      <c r="C6" s="9">
+        <v>9.849413886384129</v>
+      </c>
+      <c r="D6" s="7">
+        <v>59.546541861674456</v>
       </c>
       <c r="E6">
         <v>3.4162348877374789</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>54.099489029155393</v>
       </c>
       <c r="G6">
@@ -622,22 +633,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>360</v>
-      </c>
-      <c r="B7">
-        <v>7.3886010362694305</v>
-      </c>
-      <c r="C7" s="4">
-        <v>51.370303576795912</v>
-      </c>
-      <c r="D7">
-        <v>12.328653146125845</v>
+      <c r="A7" s="5">
+        <v>260</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2.5008635578583758</v>
+      </c>
+      <c r="C7" s="9">
+        <v>9.4286143672978664</v>
+      </c>
+      <c r="D7" s="7">
+        <v>58.516900676027035</v>
       </c>
       <c r="E7">
         <v>2.9671848013816917</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>36.492034866245866</v>
       </c>
       <c r="G7">
@@ -645,26 +656,40 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="5">
+        <v>360</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1.6718480138169254</v>
+      </c>
+      <c r="C8" s="9">
+        <v>9.651036970243462</v>
+      </c>
+      <c r="D8" s="7">
+        <v>58.964118564742584</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.585492227979274</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43.44123835287045</v>
+      </c>
+      <c r="G8" s="4">
+        <v>32.786271450858031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <v>1440</v>
       </c>
-      <c r="B8" s="3">
-        <v>3.6407599309153711</v>
-      </c>
-      <c r="C8" s="5">
-        <v>47.955816050495947</v>
-      </c>
-      <c r="D8" s="6">
-        <v>13.051482059282371</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.585492227979274</v>
-      </c>
-      <c r="F8" s="5">
-        <v>43.44123835287045</v>
-      </c>
-      <c r="G8" s="6">
-        <v>32.786271450858031</v>
+      <c r="B9" s="8">
+        <v>-0.21070811744386872</v>
+      </c>
+      <c r="C9" s="10">
+        <v>11.141869552149084</v>
+      </c>
+      <c r="D9" s="11">
+        <v>65.287571502860118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug: The measured data is not correct! The 0 value has to be ignored!
</commit_message>
<xml_diff>
--- a/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
+++ b/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMalz\Desktop\Repos\wt_modeling\Drafts\lmfit_biocatalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E6F62A-7FC8-455E-AE4F-DAFC47B5D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF21E467-3437-4244-8561-ECC506E1EDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58290" yWindow="11325" windowWidth="15705" windowHeight="9720" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B764C8B-F5EC-4044-AE1A-6A1FF61ED92C}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="F13" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,176 +519,153 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7">
-        <v>118.42487046632124</v>
+        <v>34.936096718480137</v>
       </c>
       <c r="C2" s="9">
-        <v>0.14697926059513075</v>
+        <v>21.932371505861141</v>
       </c>
       <c r="D2" s="7">
-        <v>8.736349453978158E-2</v>
+        <v>16.15600624024961</v>
       </c>
       <c r="E2">
-        <v>132.84628670120895</v>
+        <v>37.146804835924009</v>
       </c>
       <c r="F2" s="2">
-        <v>0.14697926059513075</v>
+        <v>42.250976856026455</v>
       </c>
       <c r="G2">
-        <v>8.736349453978158E-2</v>
+        <v>2.937077483099324</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7">
-        <v>34.936096718480137</v>
+        <v>12.690846286701209</v>
       </c>
       <c r="C3" s="9">
-        <v>21.932371505861141</v>
+        <v>19.684099789600243</v>
       </c>
       <c r="D3" s="7">
-        <v>16.15600624024961</v>
+        <v>41.751430057202278</v>
       </c>
       <c r="E3">
-        <v>37.146804835924009</v>
+        <v>22.656303972366146</v>
       </c>
       <c r="F3" s="2">
-        <v>42.250976856026455</v>
+        <v>46.116321009918842</v>
       </c>
       <c r="G3">
-        <v>2.937077483099324</v>
+        <v>3.6235049401976078</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B4" s="7">
-        <v>12.690846286701209</v>
+        <v>6.3350604490500855</v>
       </c>
       <c r="C4" s="9">
-        <v>19.684099789600243</v>
+        <v>11.424406372107002</v>
       </c>
       <c r="D4" s="7">
-        <v>41.751430057202278</v>
+        <v>54.491939677587091</v>
       </c>
       <c r="E4">
-        <v>22.656303972366146</v>
+        <v>11.930915371329879</v>
       </c>
       <c r="F4" s="2">
-        <v>46.116321009918842</v>
+        <v>44.421100090171329</v>
       </c>
       <c r="G4">
-        <v>3.6235049401976078</v>
+        <v>10.799791991679667</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5" s="7">
-        <v>6.3350604490500855</v>
+        <v>4.7288428324697742</v>
       </c>
       <c r="C5" s="9">
-        <v>11.424406372107002</v>
+        <v>9.849413886384129</v>
       </c>
       <c r="D5" s="7">
-        <v>54.491939677587091</v>
+        <v>59.546541861674456</v>
       </c>
       <c r="E5">
-        <v>11.930915371329879</v>
+        <v>3.4162348877374789</v>
       </c>
       <c r="F5" s="2">
-        <v>44.421100090171329</v>
+        <v>54.099489029155393</v>
       </c>
       <c r="G5">
-        <v>10.799791991679667</v>
+        <v>32.079043161726467</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="B6" s="7">
-        <v>4.7288428324697742</v>
+        <v>2.5008635578583758</v>
       </c>
       <c r="C6" s="9">
-        <v>9.849413886384129</v>
+        <v>9.4286143672978664</v>
       </c>
       <c r="D6" s="7">
-        <v>59.546541861674456</v>
+        <v>58.516900676027035</v>
       </c>
       <c r="E6">
-        <v>3.4162348877374789</v>
+        <v>2.9671848013816917</v>
       </c>
       <c r="F6" s="2">
-        <v>54.099489029155393</v>
+        <v>36.492034866245866</v>
       </c>
       <c r="G6">
-        <v>32.079043161726467</v>
+        <v>24.205928237129484</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="B7" s="7">
-        <v>2.5008635578583758</v>
+        <v>1.6718480138169254</v>
       </c>
       <c r="C7" s="9">
-        <v>9.4286143672978664</v>
+        <v>9.651036970243462</v>
       </c>
       <c r="D7" s="7">
-        <v>58.516900676027035</v>
-      </c>
-      <c r="E7">
-        <v>2.9671848013816917</v>
-      </c>
-      <c r="F7" s="2">
-        <v>36.492034866245866</v>
-      </c>
-      <c r="G7">
-        <v>24.205928237129484</v>
+        <v>58.964118564742584</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.585492227979274</v>
+      </c>
+      <c r="F7" s="3">
+        <v>43.44123835287045</v>
+      </c>
+      <c r="G7" s="4">
+        <v>32.786271450858031</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>360</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1.6718480138169254</v>
-      </c>
-      <c r="C8" s="9">
-        <v>9.651036970243462</v>
-      </c>
-      <c r="D8" s="7">
-        <v>58.964118564742584</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1.585492227979274</v>
-      </c>
-      <c r="F8" s="3">
-        <v>43.44123835287045</v>
-      </c>
-      <c r="G8" s="4">
-        <v>32.786271450858031</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A8" s="6">
         <v>1440</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B8" s="8">
         <v>-0.21070811744386872</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C8" s="10">
         <v>11.141869552149084</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D8" s="11">
         <v>65.287571502860118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: dominic data added
</commit_message>
<xml_diff>
--- a/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
+++ b/Drafts/lmfit_biocatalysis/Jan_Carina_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMalz\Desktop\Repos\wt_modeling\Drafts\lmfit_biocatalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF21E467-3437-4244-8561-ECC506E1EDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E2191C-DD86-4829-B076-AB14A48822EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
+    <workbookView xWindow="58665" yWindow="8925" windowWidth="15705" windowHeight="9720" xr2:uid="{F692BA46-C83B-41D0-94DB-A9CC2E210C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Zeit</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>Octandiol-400</t>
+  </si>
+  <si>
+    <t>Butanal-50p</t>
+  </si>
+  <si>
+    <t>Butyroin-50p</t>
+  </si>
+  <si>
+    <t>Octandiol-50p</t>
+  </si>
+  <si>
+    <t>Butanal-20</t>
+  </si>
+  <si>
+    <t>Butyroin-20</t>
+  </si>
+  <si>
+    <t>Octandiol-20</t>
   </si>
 </sst>
 </file>
@@ -483,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B764C8B-F5EC-4044-AE1A-6A1FF61ED92C}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F12:F13"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +512,7 @@
     <col min="4" max="4" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,158 +534,314 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>15</v>
       </c>
-      <c r="B2" s="7">
-        <v>34.936096718480137</v>
-      </c>
-      <c r="C2" s="9">
-        <v>21.932371505861141</v>
-      </c>
-      <c r="D2" s="7">
-        <v>16.15600624024961</v>
+      <c r="B2">
+        <v>124.1761658031088</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15.794709948902915</v>
+      </c>
+      <c r="D2">
+        <v>4.7571502860114405</v>
       </c>
       <c r="E2">
-        <v>37.146804835924009</v>
+        <v>28.994818652849744</v>
       </c>
       <c r="F2" s="2">
-        <v>42.250976856026455</v>
+        <v>36.017132551848512</v>
       </c>
       <c r="G2">
-        <v>2.937077483099324</v>
+        <v>11.694227769110762</v>
+      </c>
+      <c r="H2" s="7">
+        <v>71.550949913644203</v>
+      </c>
+      <c r="I2" s="9">
+        <v>13.744815148782687</v>
+      </c>
+      <c r="J2" s="7">
+        <v>5.4123764950598021</v>
+      </c>
+      <c r="K2">
+        <v>59.927461139896366</v>
+      </c>
+      <c r="L2" s="2">
+        <v>44.956116621581003</v>
+      </c>
+      <c r="M2">
+        <v>8.736349453978158E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>30</v>
       </c>
-      <c r="B3" s="7">
-        <v>12.690846286701209</v>
-      </c>
-      <c r="C3" s="9">
-        <v>19.684099789600243</v>
-      </c>
-      <c r="D3" s="7">
-        <v>41.751430057202278</v>
+      <c r="B3">
+        <v>63.398963730569939</v>
+      </c>
+      <c r="C3" s="2">
+        <v>25.996092575894199</v>
+      </c>
+      <c r="D3">
+        <v>17.757670306812273</v>
       </c>
       <c r="E3">
-        <v>22.656303972366146</v>
+        <v>11.689119170984457</v>
       </c>
       <c r="F3" s="2">
-        <v>46.116321009918842</v>
+        <v>40.381424706943193</v>
       </c>
       <c r="G3">
-        <v>3.6235049401976078</v>
+        <v>24.434737389495581</v>
+      </c>
+      <c r="H3" s="7">
+        <v>27.924006908462871</v>
+      </c>
+      <c r="I3" s="9">
+        <v>18.950706342049894</v>
+      </c>
+      <c r="J3" s="7">
+        <v>21.574622984919397</v>
+      </c>
+      <c r="K3">
+        <v>32.483592400690846</v>
+      </c>
+      <c r="L3" s="2">
+        <v>52.241959723474615</v>
+      </c>
+      <c r="M3">
+        <v>1.2522100884035361</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>60</v>
       </c>
-      <c r="B4" s="7">
-        <v>6.3350604490500855</v>
-      </c>
-      <c r="C4" s="9">
-        <v>11.424406372107002</v>
-      </c>
-      <c r="D4" s="7">
-        <v>54.491939677587091</v>
+      <c r="B4">
+        <v>28.390328151986182</v>
+      </c>
+      <c r="C4" s="2">
+        <v>23.062518785692816</v>
+      </c>
+      <c r="D4">
+        <v>41.553822152886113</v>
       </c>
       <c r="E4">
-        <v>11.930915371329879</v>
+        <v>4.1934369602763386</v>
       </c>
       <c r="F4" s="2">
-        <v>44.421100090171329</v>
+        <v>31.520589119326726</v>
       </c>
       <c r="G4">
-        <v>10.799791991679667</v>
+        <v>37.695267810712416</v>
+      </c>
+      <c r="H4" s="7">
+        <v>13.727115716753024</v>
+      </c>
+      <c r="I4" s="9">
+        <v>15.488127442140067</v>
+      </c>
+      <c r="J4" s="7">
+        <v>47.128445137805507</v>
+      </c>
+      <c r="K4">
+        <v>14.21070811744387</v>
+      </c>
+      <c r="L4" s="2">
+        <v>50.035767959122332</v>
+      </c>
+      <c r="M4">
+        <v>2.7706708268330726</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>120</v>
       </c>
-      <c r="B5" s="7">
-        <v>4.7288428324697742</v>
-      </c>
-      <c r="C5" s="9">
-        <v>9.849413886384129</v>
-      </c>
-      <c r="D5" s="7">
-        <v>59.546541861674456</v>
+      <c r="B5">
+        <v>10.756476683937825</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12.852119026149685</v>
+      </c>
+      <c r="D5">
+        <v>70.238169526781078</v>
       </c>
       <c r="E5">
-        <v>3.4162348877374789</v>
+        <v>2.8981001727115712</v>
       </c>
       <c r="F5" s="2">
-        <v>54.099489029155393</v>
+        <v>27.030057108506167</v>
       </c>
       <c r="G5">
-        <v>32.079043161726467</v>
+        <v>45.349973998959946</v>
+      </c>
+      <c r="H5" s="7">
+        <v>7.6476683937823822</v>
+      </c>
+      <c r="I5" s="9">
+        <v>7.9377817853922457</v>
+      </c>
+      <c r="J5" s="7">
+        <v>66.535621424856984</v>
+      </c>
+      <c r="K5">
+        <v>11.326424870466321</v>
+      </c>
+      <c r="L5" s="2">
+        <v>68.722272317403068</v>
+      </c>
+      <c r="M5">
+        <v>6.4940197607904322</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>260</v>
       </c>
-      <c r="B6" s="7">
-        <v>2.5008635578583758</v>
-      </c>
-      <c r="C6" s="9">
-        <v>9.4286143672978664</v>
-      </c>
-      <c r="D6" s="7">
-        <v>58.516900676027035</v>
+      <c r="B6">
+        <v>5.6960276338514682</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6.6453261196272919</v>
+      </c>
+      <c r="D6">
+        <v>77.924076963078519</v>
       </c>
       <c r="E6">
-        <v>2.9671848013816917</v>
+        <v>0.67012089810017261</v>
       </c>
       <c r="F6" s="2">
-        <v>36.492034866245866</v>
+        <v>28.328524195972349</v>
       </c>
       <c r="G6">
-        <v>24.205928237129484</v>
+        <v>51.673426937077473</v>
+      </c>
+      <c r="H6" s="7">
+        <v>4.3834196891191706</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5.8097385031559972</v>
+      </c>
+      <c r="J6" s="7">
+        <v>70.456578263130538</v>
+      </c>
+      <c r="K6">
+        <v>4.9706390328151979</v>
+      </c>
+      <c r="L6" s="2">
+        <v>52.109708446047499</v>
+      </c>
+      <c r="M6">
+        <v>9.0629225169006755</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>360</v>
       </c>
-      <c r="B7" s="7">
-        <v>1.6718480138169254</v>
-      </c>
-      <c r="C7" s="9">
-        <v>9.651036970243462</v>
-      </c>
-      <c r="D7" s="7">
-        <v>58.964118564742584</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1.585492227979274</v>
-      </c>
-      <c r="F7" s="3">
-        <v>43.44123835287045</v>
-      </c>
-      <c r="G7" s="4">
-        <v>32.786271450858031</v>
+      <c r="B7">
+        <v>4.0725388601036263</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.893898406973249</v>
+      </c>
+      <c r="D7">
+        <v>84.715548621944876</v>
+      </c>
+      <c r="E7">
+        <v>-0.84974093264248696</v>
+      </c>
+      <c r="F7" s="2">
+        <v>26.30267508265705</v>
+      </c>
+      <c r="G7">
+        <v>48.854914196567854</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3.1053540587219337</v>
+      </c>
+      <c r="I7" s="9">
+        <v>5.0042079951908622</v>
+      </c>
+      <c r="J7" s="7">
+        <v>64.580343213728554</v>
+      </c>
+      <c r="K7">
+        <v>7.3886010362694305</v>
+      </c>
+      <c r="L7" s="2">
+        <v>51.370303576795912</v>
+      </c>
+      <c r="M7">
+        <v>12.328653146125845</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1440</v>
       </c>
-      <c r="B8" s="8">
-        <v>-0.21070811744386872</v>
-      </c>
-      <c r="C8" s="10">
-        <v>11.141869552149084</v>
-      </c>
-      <c r="D8" s="11">
-        <v>65.287571502860118</v>
-      </c>
+      <c r="B8" s="1">
+        <v>1.4473229706390329</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.4851217312894498</v>
+      </c>
+      <c r="D8" s="4">
+        <v>85.98439937597503</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-1.0051813471502591</v>
+      </c>
+      <c r="F8" s="3">
+        <v>25.629395852119028</v>
+      </c>
+      <c r="G8" s="4">
+        <v>53.597503900155999</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.2918825561312606</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5.9660354673880365</v>
+      </c>
+      <c r="J8" s="11">
+        <v>75.542381695267807</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3.6407599309153711</v>
+      </c>
+      <c r="L8" s="3">
+        <v>47.955816050495947</v>
+      </c>
+      <c r="M8" s="4">
+        <v>13.051482059282371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>